<commit_message>
Added subject label to the front of flashcards for better organization
</commit_message>
<xml_diff>
--- a/data/unit1.xlsx
+++ b/data/unit1.xlsx
@@ -3559,10 +3559,10 @@
         </is>
       </c>
       <c r="E128" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F128" s="2" t="n">
-        <v>45736</v>
+        <v>45739</v>
       </c>
     </row>
     <row r="129">

</xml_diff>